<commit_message>
add more question at kpop:
</commit_message>
<xml_diff>
--- a/Questions/Kpop.xlsx
+++ b/Questions/Kpop.xlsx
@@ -8,9 +8,9 @@
       <x15ac:absPath xmlns:x15ac="http://schemas.microsoft.com/office/spreadsheetml/2010/11/ac" url="/Users/jun/My Works/Rails/speedQuizRails/Questions/"/>
     </mc:Choice>
   </mc:AlternateContent>
-  <xr:revisionPtr revIDLastSave="0" documentId="13_ncr:1_{9CD3918D-07A7-5D47-9B0F-1A12AC38426B}" xr6:coauthVersionLast="45" xr6:coauthVersionMax="45" xr10:uidLastSave="{00000000-0000-0000-0000-000000000000}"/>
+  <xr:revisionPtr revIDLastSave="0" documentId="13_ncr:1_{7C6C6AD3-2565-6248-9A8B-CE8E264B5B4D}" xr6:coauthVersionLast="45" xr6:coauthVersionMax="45" xr10:uidLastSave="{00000000-0000-0000-0000-000000000000}"/>
   <bookViews>
-    <workbookView xWindow="0" yWindow="500" windowWidth="28800" windowHeight="17500" xr2:uid="{FCFFE160-7E7A-7D43-884F-B1C8E6562C0E}"/>
+    <workbookView xWindow="28800" yWindow="3140" windowWidth="19200" windowHeight="14860" xr2:uid="{FCFFE160-7E7A-7D43-884F-B1C8E6562C0E}"/>
   </bookViews>
   <sheets>
     <sheet name="Sheet1" sheetId="1" r:id="rId1"/>
@@ -34,7 +34,7 @@
 </file>
 
 <file path=xl/sharedStrings.xml><?xml version="1.0" encoding="utf-8"?>
-<sst xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" count="85" uniqueCount="84">
+<sst xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" count="118" uniqueCount="117">
   <si>
     <t>id</t>
   </si>
@@ -271,9 +271,6 @@
     <t>OxgiiyLp5pk</t>
   </si>
   <si>
-    <t>k5WqGIPjqtc</t>
-  </si>
-  <si>
     <t>dEIULaQgGiQ</t>
   </si>
   <si>
@@ -326,11 +323,129 @@
     <phoneticPr fontId="2" type="noConversion"/>
   </si>
   <si>
-    <t>ihnzsr9yUEI</t>
-    <phoneticPr fontId="2" type="noConversion"/>
-  </si>
-  <si>
     <t>sF9sv9lT83A</t>
+  </si>
+  <si>
+    <t>LYZ7gdFkmcs</t>
+  </si>
+  <si>
+    <t>Asmt-dgB-64</t>
+  </si>
+  <si>
+    <t>노브레인</t>
+    <phoneticPr fontId="2" type="noConversion"/>
+  </si>
+  <si>
+    <t>노라조</t>
+    <phoneticPr fontId="2" type="noConversion"/>
+  </si>
+  <si>
+    <t>kFv1IQLekU0</t>
+  </si>
+  <si>
+    <t>ao58vQDMVlQ</t>
+  </si>
+  <si>
+    <t>허각</t>
+    <phoneticPr fontId="2" type="noConversion"/>
+  </si>
+  <si>
+    <t>김필</t>
+    <phoneticPr fontId="2" type="noConversion"/>
+  </si>
+  <si>
+    <t>3xdfBwFb2DU</t>
+  </si>
+  <si>
+    <t>어반자카파</t>
+    <phoneticPr fontId="2" type="noConversion"/>
+  </si>
+  <si>
+    <t>T5_O38Bpeto</t>
+  </si>
+  <si>
+    <t>자우림</t>
+    <phoneticPr fontId="2" type="noConversion"/>
+  </si>
+  <si>
+    <t>체리필터</t>
+    <phoneticPr fontId="2" type="noConversion"/>
+  </si>
+  <si>
+    <t>fmq2k0MkZ0g</t>
+  </si>
+  <si>
+    <t>김종국</t>
+    <phoneticPr fontId="2" type="noConversion"/>
+  </si>
+  <si>
+    <t>이승기</t>
+    <phoneticPr fontId="2" type="noConversion"/>
+  </si>
+  <si>
+    <t>안예은</t>
+    <phoneticPr fontId="2" type="noConversion"/>
+  </si>
+  <si>
+    <t>qvJ1FHRR1n8</t>
+  </si>
+  <si>
+    <t>HkQ6HvW9nrA</t>
+  </si>
+  <si>
+    <t>김상민</t>
+    <phoneticPr fontId="2" type="noConversion"/>
+  </si>
+  <si>
+    <t>유리상자</t>
+    <phoneticPr fontId="2" type="noConversion"/>
+  </si>
+  <si>
+    <t>에스지워너비</t>
+    <phoneticPr fontId="2" type="noConversion"/>
+  </si>
+  <si>
+    <t>SG워너비</t>
+    <phoneticPr fontId="2" type="noConversion"/>
+  </si>
+  <si>
+    <t>zJfF_41gOk8</t>
+  </si>
+  <si>
+    <t>xhj-xbO6Yvs</t>
+  </si>
+  <si>
+    <t>xZdTzNLmCN8</t>
+  </si>
+  <si>
+    <t>LneGd_itknE</t>
+  </si>
+  <si>
+    <t>URdpWdfTlao</t>
+  </si>
+  <si>
+    <t>김태우</t>
+    <phoneticPr fontId="2" type="noConversion"/>
+  </si>
+  <si>
+    <t>pBRZzsO3L3o</t>
+  </si>
+  <si>
+    <t>토이</t>
+    <phoneticPr fontId="2" type="noConversion"/>
+  </si>
+  <si>
+    <t>swM_GL06CxM</t>
+  </si>
+  <si>
+    <t>l5BgC6iwLNA</t>
+  </si>
+  <si>
+    <t>윤하</t>
+    <phoneticPr fontId="2" type="noConversion"/>
+  </si>
+  <si>
+    <t>FZpYfZiBEaU</t>
   </si>
 </sst>
 </file>
@@ -722,10 +837,10 @@
 
 <file path=xl/worksheets/sheet1.xml><?xml version="1.0" encoding="utf-8"?>
 <worksheet xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:x14ac="http://schemas.microsoft.com/office/spreadsheetml/2009/9/ac" xmlns:xr="http://schemas.microsoft.com/office/spreadsheetml/2014/revision" xmlns:xr2="http://schemas.microsoft.com/office/spreadsheetml/2015/revision2" xmlns:xr3="http://schemas.microsoft.com/office/spreadsheetml/2016/revision3" mc:Ignorable="x14ac xr xr2 xr3" xr:uid="{8BFE90B0-B9DA-C240-8DC8-0306D80CDE5D}">
-  <dimension ref="A1:E38"/>
+  <dimension ref="A1:E54"/>
   <sheetViews>
-    <sheetView tabSelected="1" zoomScale="75" workbookViewId="0">
-      <selection activeCell="C29" sqref="C29"/>
+    <sheetView tabSelected="1" topLeftCell="A26" zoomScale="84" zoomScaleNormal="56" workbookViewId="0">
+      <selection activeCell="C55" sqref="C55"/>
     </sheetView>
   </sheetViews>
   <sheetFormatPr baseColWidth="10" defaultRowHeight="18"/>
@@ -882,7 +997,7 @@
         <v>13</v>
       </c>
       <c r="E10" t="s">
-        <v>77</v>
+        <v>76</v>
       </c>
     </row>
     <row r="11" spans="1:5">
@@ -1061,7 +1176,7 @@
         <v>22</v>
       </c>
       <c r="B23" s="2" t="s">
-        <v>70</v>
+        <v>69</v>
       </c>
       <c r="C23">
         <v>0</v>
@@ -1089,10 +1204,10 @@
         <v>24</v>
       </c>
       <c r="B25" t="s">
-        <v>65</v>
+        <v>83</v>
       </c>
       <c r="C25">
-        <v>29</v>
+        <v>68</v>
       </c>
       <c r="D25" t="s">
         <v>34</v>
@@ -1117,7 +1232,7 @@
         <v>26</v>
       </c>
       <c r="B27" t="s">
-        <v>66</v>
+        <v>65</v>
       </c>
       <c r="C27">
         <v>0</v>
@@ -1131,7 +1246,7 @@
         <v>27</v>
       </c>
       <c r="B28" t="s">
-        <v>83</v>
+        <v>81</v>
       </c>
       <c r="C28">
         <v>85</v>
@@ -1140,7 +1255,7 @@
         <v>37</v>
       </c>
       <c r="E28" t="s">
-        <v>78</v>
+        <v>77</v>
       </c>
     </row>
     <row r="29" spans="1:5">
@@ -1148,7 +1263,7 @@
         <v>28</v>
       </c>
       <c r="B29" s="3" t="s">
-        <v>67</v>
+        <v>66</v>
       </c>
       <c r="C29">
         <v>50</v>
@@ -1162,7 +1277,7 @@
         <v>29</v>
       </c>
       <c r="B30" t="s">
-        <v>68</v>
+        <v>67</v>
       </c>
       <c r="C30">
         <v>56</v>
@@ -1179,7 +1294,7 @@
         <v>30</v>
       </c>
       <c r="B31" t="s">
-        <v>69</v>
+        <v>68</v>
       </c>
       <c r="C31">
         <v>42</v>
@@ -1193,7 +1308,7 @@
         <v>31</v>
       </c>
       <c r="B32" t="s">
-        <v>71</v>
+        <v>70</v>
       </c>
       <c r="C32">
         <v>20</v>
@@ -1207,7 +1322,7 @@
         <v>32</v>
       </c>
       <c r="B33" t="s">
-        <v>72</v>
+        <v>71</v>
       </c>
       <c r="C33">
         <v>0</v>
@@ -1221,7 +1336,7 @@
         <v>33</v>
       </c>
       <c r="B34" t="s">
-        <v>73</v>
+        <v>72</v>
       </c>
       <c r="C34">
         <v>60</v>
@@ -1235,7 +1350,7 @@
         <v>34</v>
       </c>
       <c r="B35" t="s">
-        <v>74</v>
+        <v>73</v>
       </c>
       <c r="C35">
         <v>0</v>
@@ -1244,7 +1359,7 @@
         <v>45</v>
       </c>
       <c r="E35" t="s">
-        <v>81</v>
+        <v>80</v>
       </c>
     </row>
     <row r="36" spans="1:5">
@@ -1252,7 +1367,7 @@
         <v>35</v>
       </c>
       <c r="B36" t="s">
-        <v>75</v>
+        <v>74</v>
       </c>
       <c r="C36">
         <v>70</v>
@@ -1266,7 +1381,7 @@
         <v>36</v>
       </c>
       <c r="B37" t="s">
-        <v>76</v>
+        <v>75</v>
       </c>
       <c r="C37">
         <v>0</v>
@@ -1280,13 +1395,240 @@
         <v>37</v>
       </c>
       <c r="B38" t="s">
-        <v>80</v>
+        <v>79</v>
       </c>
       <c r="C38">
         <v>48</v>
       </c>
       <c r="D38" t="s">
-        <v>79</v>
+        <v>78</v>
+      </c>
+    </row>
+    <row r="39" spans="1:5">
+      <c r="A39">
+        <v>38</v>
+      </c>
+      <c r="B39" t="s">
+        <v>86</v>
+      </c>
+      <c r="C39">
+        <v>40</v>
+      </c>
+      <c r="D39" t="s">
+        <v>84</v>
+      </c>
+    </row>
+    <row r="40" spans="1:5">
+      <c r="A40">
+        <v>39</v>
+      </c>
+      <c r="B40" t="s">
+        <v>87</v>
+      </c>
+      <c r="C40">
+        <v>112</v>
+      </c>
+      <c r="D40" t="s">
+        <v>85</v>
+      </c>
+    </row>
+    <row r="41" spans="1:5">
+      <c r="A41">
+        <v>40</v>
+      </c>
+      <c r="B41" t="s">
+        <v>90</v>
+      </c>
+      <c r="C41">
+        <v>76</v>
+      </c>
+      <c r="D41" t="s">
+        <v>88</v>
+      </c>
+    </row>
+    <row r="42" spans="1:5">
+      <c r="A42">
+        <v>41</v>
+      </c>
+      <c r="B42" t="s">
+        <v>92</v>
+      </c>
+      <c r="C42">
+        <v>25</v>
+      </c>
+      <c r="D42" t="s">
+        <v>89</v>
+      </c>
+    </row>
+    <row r="43" spans="1:5">
+      <c r="A43">
+        <v>42</v>
+      </c>
+      <c r="B43" t="s">
+        <v>95</v>
+      </c>
+      <c r="C43">
+        <v>75</v>
+      </c>
+      <c r="D43" t="s">
+        <v>91</v>
+      </c>
+    </row>
+    <row r="44" spans="1:5">
+      <c r="A44">
+        <v>43</v>
+      </c>
+      <c r="B44" t="s">
+        <v>99</v>
+      </c>
+      <c r="C44">
+        <v>0</v>
+      </c>
+      <c r="D44" t="s">
+        <v>93</v>
+      </c>
+    </row>
+    <row r="45" spans="1:5">
+      <c r="A45">
+        <v>44</v>
+      </c>
+      <c r="B45" t="s">
+        <v>100</v>
+      </c>
+      <c r="C45">
+        <v>18</v>
+      </c>
+      <c r="D45" t="s">
+        <v>94</v>
+      </c>
+    </row>
+    <row r="46" spans="1:5">
+      <c r="A46">
+        <v>45</v>
+      </c>
+      <c r="B46" t="s">
+        <v>105</v>
+      </c>
+      <c r="C46">
+        <v>13</v>
+      </c>
+      <c r="D46" t="s">
+        <v>96</v>
+      </c>
+    </row>
+    <row r="47" spans="1:5">
+      <c r="A47">
+        <v>46</v>
+      </c>
+      <c r="B47" t="s">
+        <v>106</v>
+      </c>
+      <c r="C47">
+        <v>58</v>
+      </c>
+      <c r="D47" t="s">
+        <v>97</v>
+      </c>
+    </row>
+    <row r="48" spans="1:5">
+      <c r="A48">
+        <v>47</v>
+      </c>
+      <c r="B48" t="s">
+        <v>107</v>
+      </c>
+      <c r="C48">
+        <v>75</v>
+      </c>
+      <c r="D48" t="s">
+        <v>98</v>
+      </c>
+    </row>
+    <row r="49" spans="1:5">
+      <c r="A49">
+        <v>48</v>
+      </c>
+      <c r="B49" t="s">
+        <v>108</v>
+      </c>
+      <c r="C49">
+        <v>55</v>
+      </c>
+      <c r="D49" t="s">
+        <v>101</v>
+      </c>
+    </row>
+    <row r="50" spans="1:5">
+      <c r="A50">
+        <v>49</v>
+      </c>
+      <c r="B50" t="s">
+        <v>109</v>
+      </c>
+      <c r="C50">
+        <v>63</v>
+      </c>
+      <c r="D50" t="s">
+        <v>102</v>
+      </c>
+    </row>
+    <row r="51" spans="1:5">
+      <c r="A51">
+        <v>50</v>
+      </c>
+      <c r="B51" t="s">
+        <v>113</v>
+      </c>
+      <c r="C51">
+        <v>78</v>
+      </c>
+      <c r="D51" t="s">
+        <v>103</v>
+      </c>
+      <c r="E51" t="s">
+        <v>104</v>
+      </c>
+    </row>
+    <row r="52" spans="1:5">
+      <c r="A52">
+        <v>51</v>
+      </c>
+      <c r="B52" t="s">
+        <v>114</v>
+      </c>
+      <c r="C52">
+        <v>0</v>
+      </c>
+      <c r="D52" t="s">
+        <v>110</v>
+      </c>
+    </row>
+    <row r="53" spans="1:5">
+      <c r="A53">
+        <v>52</v>
+      </c>
+      <c r="B53" t="s">
+        <v>111</v>
+      </c>
+      <c r="C53">
+        <v>75</v>
+      </c>
+      <c r="D53" t="s">
+        <v>112</v>
+      </c>
+    </row>
+    <row r="54" spans="1:5">
+      <c r="A54">
+        <v>53</v>
+      </c>
+      <c r="B54" t="s">
+        <v>116</v>
+      </c>
+      <c r="C54">
+        <v>0</v>
+      </c>
+      <c r="D54" t="s">
+        <v>115</v>
       </c>
     </row>
   </sheetData>

</xml_diff>